<commit_message>
Updated symbols/footprint for USB and 5K Trimmer Pots.
</commit_message>
<xml_diff>
--- a/cpu.xlsx
+++ b/cpu.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prj\youtube\ian_ward\homebrew_cpu\Homebrew CPU PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prj\yt\ian_ward\homebrew_cpu\Homebrew-CPU-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BCBC9C7F-4440-42D1-9DBF-789BCF28F264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053768AC-08BB-4ECA-9528-EAB0D88D8718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="13952"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="13952" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="cpu" sheetId="1" r:id="rId1"/>
+    <sheet name="_cpu" sheetId="1" r:id="rId1"/>
+    <sheet name="cpu" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="82">
   <si>
     <t>#</t>
   </si>
@@ -290,11 +291,20 @@
   <si>
     <t>Jameco</t>
   </si>
+  <si>
+    <t>Vendor\Part #</t>
+  </si>
+  <si>
+    <t>Vendor URL</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1181,11 +1191,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1740,31 +1750,84 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G12" r:id="rId1"/>
-    <hyperlink ref="H12" r:id="rId2"/>
-    <hyperlink ref="G18" r:id="rId3"/>
-    <hyperlink ref="H18" r:id="rId4"/>
-    <hyperlink ref="G20" r:id="rId5"/>
-    <hyperlink ref="H20" r:id="rId6"/>
-    <hyperlink ref="G21" r:id="rId7"/>
-    <hyperlink ref="H21" r:id="rId8"/>
-    <hyperlink ref="G22" r:id="rId9"/>
-    <hyperlink ref="H22" r:id="rId10"/>
-    <hyperlink ref="G23" r:id="rId11"/>
-    <hyperlink ref="H23" r:id="rId12"/>
-    <hyperlink ref="G27" r:id="rId13"/>
-    <hyperlink ref="H27" r:id="rId14"/>
-    <hyperlink ref="G24" r:id="rId15"/>
-    <hyperlink ref="H24" r:id="rId16"/>
-    <hyperlink ref="G25" r:id="rId17"/>
-    <hyperlink ref="H25" r:id="rId18"/>
-    <hyperlink ref="G26" r:id="rId19"/>
-    <hyperlink ref="H26" r:id="rId20"/>
-    <hyperlink ref="G19" r:id="rId21"/>
-    <hyperlink ref="H19" r:id="rId22"/>
-    <hyperlink ref="G11" r:id="rId23"/>
-    <hyperlink ref="H11" r:id="rId24"/>
+    <hyperlink ref="G12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G18" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H18" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G20" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H20" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G21" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H21" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G22" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H22" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G23" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H23" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G27" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H27" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G24" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H24" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G25" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H25" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G26" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="H26" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G19" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="H19" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G11" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="H11" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C382D7-551C-4DB5-967D-4304CEB98B2E}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="25.875" customWidth="1"/>
+    <col min="5" max="5" width="36.625" customWidth="1"/>
+    <col min="6" max="6" width="37.625" customWidth="1"/>
+    <col min="7" max="7" width="31.5" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
+    <col min="9" max="9" width="26.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>